<commit_message>
add option to return focus on windows restore
</commit_message>
<xml_diff>
--- a/language_gen/language_gen.xlsx
+++ b/language_gen/language_gen.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
   <si>
     <t>HEADER</t>
   </si>
@@ -71,6 +71,12 @@
   </si>
   <si>
     <t>Save legacy windows</t>
+  </si>
+  <si>
+    <t>TextId_Tray_Opt_Restore_Focus</t>
+  </si>
+  <si>
+    <t>Return focus to restored windows</t>
   </si>
   <si>
     <t>TextId_Tray_Edit_Hotkeys</t>
@@ -546,15 +552,15 @@
       </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -562,7 +568,7 @@
       </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -570,22 +576,22 @@
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
-      <c r="B13" s="1"/>
+      <c r="A13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="B14" s="1"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="2" t="s">
-        <v>27</v>
+      <c r="A15" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
@@ -677,8 +683,12 @@
       </c>
     </row>
     <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" s="6"/>
-      <c r="B27" s="1"/>
+      <c r="A27" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="6"/>
@@ -794,26 +804,25 @@
     </row>
     <row r="56" ht="14.25" customHeight="1">
       <c r="A56" s="6"/>
-      <c r="B56" s="8"/>
-      <c r="C56" s="8"/>
+      <c r="B56" s="1"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="6"/>
-      <c r="B57" s="1"/>
+      <c r="B57" s="8"/>
+      <c r="C57" s="8"/>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="6"/>
-      <c r="B58" s="8"/>
-      <c r="C58" s="8"/>
+      <c r="B58" s="1"/>
     </row>
     <row r="59" ht="14.25" customHeight="1">
       <c r="A59" s="6"/>
-      <c r="B59" s="1"/>
+      <c r="B59" s="8"/>
+      <c r="C59" s="8"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="6"/>
-      <c r="B60" s="8"/>
-      <c r="C60" s="8"/>
+      <c r="B60" s="1"/>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="6"/>
@@ -822,7 +831,8 @@
     </row>
     <row r="62" ht="14.25" customHeight="1">
       <c r="A62" s="6"/>
-      <c r="B62" s="1"/>
+      <c r="B62" s="8"/>
+      <c r="C62" s="8"/>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="6"/>
@@ -870,12 +880,12 @@
     </row>
     <row r="74" ht="14.25" customHeight="1">
       <c r="A74" s="6"/>
-      <c r="B74" s="8"/>
-      <c r="C74" s="8"/>
+      <c r="B74" s="1"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="6"/>
-      <c r="B75" s="1"/>
+      <c r="B75" s="8"/>
+      <c r="C75" s="8"/>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="6"/>
@@ -4576,6 +4586,10 @@
     <row r="1000" ht="14.25" customHeight="1">
       <c r="A1000" s="6"/>
       <c r="B1000" s="1"/>
+    </row>
+    <row r="1001" ht="14.25" customHeight="1">
+      <c r="A1001" s="6"/>
+      <c r="B1001" s="1"/>
     </row>
   </sheetData>
   <printOptions/>

</xml_diff>